<commit_message>
Online version and cost button
</commit_message>
<xml_diff>
--- a/Data/SDE_Warmte_Brabant.xlsx
+++ b/Data/SDE_Warmte_Brabant.xlsx
@@ -1,16 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s124129\Documents\GitHub\Brabant-systeem-integratie-model\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB407B2B-EEEF-4614-B211-58C5A599B58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet name="SDE_Warmte_Brabant" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="SDE_Warmte_Brabant" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="635">
   <si>
     <t>Naam</t>
   </si>
@@ -36,12 +57,6 @@
     <t>SubSoort</t>
   </si>
   <si>
-    <t>V_MW</t>
-  </si>
-  <si>
-    <t>E_MWhpa</t>
-  </si>
-  <si>
     <t>color</t>
   </si>
   <si>
@@ -51,6 +66,12 @@
     <t>wkt</t>
   </si>
   <si>
+    <t>xcoord</t>
+  </si>
+  <si>
+    <t>ycoord</t>
+  </si>
+  <si>
     <t>SDE1515275 Biomassa</t>
   </si>
   <si>
@@ -1909,34 +1930,35 @@
   </si>
   <si>
     <t>POINT (5.2090761 51.694986)</t>
+  </si>
+  <si>
+    <t>V_MWth</t>
+  </si>
+  <si>
+    <t>E_Mwhpa (th)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="DD/MM/YY" numFmtId="165"/>
-    <numFmt formatCode="DD/MM/YYYY\ HH:MM:SS" numFmtId="166"/>
-    <numFmt formatCode="HH:MM:SS" numFmtId="167"/>
-    <numFmt formatCode="DD/MM/YYYY\ HH:MM:SS.000" numFmtId="168"/>
-    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="169"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
     </font>
   </fonts>
-  <fills count="1">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1945,42 +1967,369 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="164">
-</xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="164" xfId="0"/>
-    <xf numFmtId="165" xfId="0"/>
-    <xf numFmtId="166" xfId="0"/>
-    <xf numFmtId="167" xfId="0"/>
-    <xf numFmtId="168" xfId="0"/>
-    <xf numFmtId="169" xfId="0"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E14304D3-0A89-414F-8DC3-1043512733EE}" name="Table1" displayName="Table1" ref="A1:O165" totalsRowShown="0">
+  <autoFilter ref="A1:O165" xr:uid="{E14304D3-0A89-414F-8DC3-1043512733EE}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="aardWarmte"/>
+        <filter val="bioGas"/>
+        <filter val="bioWarmte"/>
+        <filter val="zonneWarmte"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{F1676507-0C42-4C11-A708-984C98B2BB76}" name="Naam"/>
+    <tableColumn id="2" xr3:uid="{2E2ADA70-F1CF-4BD1-8A1C-214F41761338}" name="popup"/>
+    <tableColumn id="3" xr3:uid="{5DAA559D-7521-4F78-8B58-FC1DFC76DC1F}" name="Budget"/>
+    <tableColumn id="4" xr3:uid="{B8286485-8DBC-460B-8E98-5DD967FFB1EB}" name="Status"/>
+    <tableColumn id="5" xr3:uid="{26EBC639-F501-4011-8010-EEED87769C66}" name="Beschik_jr"/>
+    <tableColumn id="6" xr3:uid="{799E25E8-3111-482E-A4B9-3A21EABEC625}" name="Bouw_jr"/>
+    <tableColumn id="7" xr3:uid="{09513B29-3C11-4F0C-AE7D-202EB9B67B58}" name="Soort"/>
+    <tableColumn id="8" xr3:uid="{88CEA0D3-8AEA-47C1-947D-939509A7D2D5}" name="SubSoort"/>
+    <tableColumn id="9" xr3:uid="{DBD8969E-97BA-4AA3-8494-5B73F649E92F}" name="V_MWth"/>
+    <tableColumn id="10" xr3:uid="{695B7C1E-8A1E-4E6F-849A-D5EC1344FC75}" name="E_Mwhpa (th)"/>
+    <tableColumn id="11" xr3:uid="{0D54A9A5-BA15-4C1B-9ACF-0BF01F05A53C}" name="color"/>
+    <tableColumn id="12" xr3:uid="{A39243BA-2235-4DBE-91FC-B75A829D8216}" name="radius"/>
+    <tableColumn id="13" xr3:uid="{734ECBDD-BCF8-4193-9E4A-1E1D4B1C8CEC}" name="wkt"/>
+    <tableColumn id="14" xr3:uid="{536227CB-7115-4A99-B3E6-485CB3B0937B}" name="xcoord"/>
+    <tableColumn id="15" xr3:uid="{E3106B11-AB3E-422A-9B52-53D72D3A2363}" name="ycoord"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O165"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:O165"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1024" width="15"/>
-    <col min="2" max="1024" width="15"/>
-    <col min="3" max="1024" width="15"/>
-    <col min="4" max="1024" width="15"/>
-    <col min="5" max="1024" width="15"/>
-    <col min="6" max="1024" width="15"/>
-    <col min="7" max="1024" width="15"/>
-    <col min="8" max="1024" width="15"/>
-    <col min="9" max="1024" width="15"/>
-    <col min="10" max="1024" width="15"/>
-    <col min="11" max="1024" width="15"/>
-    <col min="12" max="1024" width="15"/>
-    <col min="13" max="1024" width="15"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2006,22 +2355,28 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>633</v>
+      </c>
+      <c r="J1" t="s">
+        <v>634</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2047,7 +2402,7 @@
         <v>18</v>
       </c>
       <c r="I2">
-        <v>37.8</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="J2">
         <v>302400</v>
@@ -2061,8 +2416,14 @@
       <c r="M2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="N2">
+        <v>4.5798263317076797</v>
+      </c>
+      <c r="O2">
+        <v>51.682658008186763</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2088,7 +2449,7 @@
         <v>24</v>
       </c>
       <c r="I3">
-        <v>29.3083</v>
+        <v>29.308299999999999</v>
       </c>
       <c r="J3">
         <v>234466.59</v>
@@ -2102,8 +2463,14 @@
       <c r="M3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="N3">
+        <v>5.6078613221650899</v>
+      </c>
+      <c r="O3">
+        <v>51.342403007905688</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -2129,7 +2496,7 @@
         <v>18</v>
       </c>
       <c r="I4">
-        <v>82.86499999999999</v>
+        <v>82.864999999999995</v>
       </c>
       <c r="J4">
         <v>344484.21</v>
@@ -2143,8 +2510,14 @@
       <c r="M4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="N4">
+        <v>5.8595619234267584</v>
+      </c>
+      <c r="O4">
+        <v>51.756540003775143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -2170,7 +2543,7 @@
         <v>35</v>
       </c>
       <c r="I5">
-        <v>9.699999999999999</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="J5">
         <v>67900</v>
@@ -2184,8 +2557,14 @@
       <c r="M5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6">
+      <c r="N5">
+        <v>5.0582895275370596</v>
+      </c>
+      <c r="O5">
+        <v>51.606745006728353</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -2225,8 +2604,14 @@
       <c r="M6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7">
+      <c r="N6">
+        <v>5.7464412214370144</v>
+      </c>
+      <c r="O6">
+        <v>51.380442007432237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -2252,7 +2637,7 @@
         <v>24</v>
       </c>
       <c r="I7">
-        <v>8.304</v>
+        <v>8.3040000000000003</v>
       </c>
       <c r="J7">
         <v>66432.22</v>
@@ -2266,8 +2651,14 @@
       <c r="M7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8">
+      <c r="N7">
+        <v>5.4525330244423023</v>
+      </c>
+      <c r="O7">
+        <v>51.510426007162309</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -2307,8 +2698,14 @@
       <c r="M8" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="9">
+      <c r="N8">
+        <v>5.745882323566744</v>
+      </c>
+      <c r="O8">
+        <v>51.662508004962532</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -2334,7 +2731,7 @@
         <v>24</v>
       </c>
       <c r="I9">
-        <v>7.3173</v>
+        <v>7.3173000000000004</v>
       </c>
       <c r="J9">
         <v>58538.55</v>
@@ -2348,8 +2745,14 @@
       <c r="M9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10">
+      <c r="N9">
+        <v>5.0582895275370596</v>
+      </c>
+      <c r="O9">
+        <v>51.606745006728353</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -2375,7 +2778,7 @@
         <v>35</v>
       </c>
       <c r="I10">
-        <v>8.208</v>
+        <v>8.2080000000000002</v>
       </c>
       <c r="J10">
         <v>57456</v>
@@ -2389,8 +2792,14 @@
       <c r="M10" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11">
+      <c r="N10">
+        <v>5.7196069232822344</v>
+      </c>
+      <c r="O10">
+        <v>51.648575005105251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -2416,7 +2825,7 @@
         <v>18</v>
       </c>
       <c r="I11">
-        <v>9.851000000000001</v>
+        <v>9.8510000000000009</v>
       </c>
       <c r="J11">
         <v>56748.72</v>
@@ -2430,8 +2839,14 @@
       <c r="M11" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="12">
+      <c r="N11">
+        <v>5.8321875230360138</v>
+      </c>
+      <c r="O11">
+        <v>51.671553005053269</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -2471,8 +2886,14 @@
       <c r="M12" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13">
+      <c r="N12">
+        <v>5.7064459221822776</v>
+      </c>
+      <c r="O12">
+        <v>51.345315007370743</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -2512,8 +2933,14 @@
       <c r="M13" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="14">
+      <c r="N13">
+        <v>4.9507771285096442</v>
+      </c>
+      <c r="O13">
+        <v>51.549448007718667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -2553,8 +2980,14 @@
       <c r="M14" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="15">
+      <c r="N14">
+        <v>4.4417652307314492</v>
+      </c>
+      <c r="O14">
+        <v>51.547565008985721</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -2594,8 +3027,14 @@
       <c r="M15" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="16">
+      <c r="N15">
+        <v>4.8020867303899921</v>
+      </c>
+      <c r="O15">
+        <v>51.683287006773782</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -2635,8 +3074,14 @@
       <c r="M16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17">
+      <c r="N16">
+        <v>4.5798263317076797</v>
+      </c>
+      <c r="O16">
+        <v>51.682658008186763</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -2676,8 +3121,14 @@
       <c r="M17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18">
+      <c r="N17">
+        <v>5.4525330244423023</v>
+      </c>
+      <c r="O17">
+        <v>51.510426007162309</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>85</v>
       </c>
@@ -2717,8 +3168,14 @@
       <c r="M18" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="19">
+      <c r="N18">
+        <v>5.6856872228720503</v>
+      </c>
+      <c r="O18">
+        <v>51.463592006340917</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>89</v>
       </c>
@@ -2758,8 +3215,14 @@
       <c r="M19" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="20">
+      <c r="N19">
+        <v>4.929876629076718</v>
+      </c>
+      <c r="O19">
+        <v>51.572970007626722</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>93</v>
       </c>
@@ -2788,7 +3251,7 @@
         <v>11.7233</v>
       </c>
       <c r="J20">
-        <v>93782.39999999999</v>
+        <v>93782.399999999994</v>
       </c>
       <c r="K20" t="s">
         <v>25</v>
@@ -2799,8 +3262,14 @@
       <c r="M20" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="21">
+      <c r="N20">
+        <v>5.5315003260124342</v>
+      </c>
+      <c r="O20">
+        <v>51.69526300514012</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>97</v>
       </c>
@@ -2840,8 +3309,14 @@
       <c r="M21" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="22">
+      <c r="N21">
+        <v>4.7915314303878764</v>
+      </c>
+      <c r="O21">
+        <v>51.729838006938458</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -2881,8 +3356,14 @@
       <c r="M22" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="23">
+      <c r="N22">
+        <v>4.415466331781972</v>
+      </c>
+      <c r="O22">
+        <v>51.626308008273618</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>107</v>
       </c>
@@ -2922,8 +3403,14 @@
       <c r="M23" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24">
+      <c r="N23">
+        <v>5.4525330244423023</v>
+      </c>
+      <c r="O23">
+        <v>51.510426007162309</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>110</v>
       </c>
@@ -2963,8 +3450,14 @@
       <c r="M24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25">
+      <c r="N24">
+        <v>4.5798263317076797</v>
+      </c>
+      <c r="O24">
+        <v>51.682658008186763</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>113</v>
       </c>
@@ -3004,8 +3497,14 @@
       <c r="M25" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="26">
+      <c r="N25">
+        <v>4.6184043308343963</v>
+      </c>
+      <c r="O25">
+        <v>51.634436008248343</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>117</v>
       </c>
@@ -3045,8 +3544,14 @@
       <c r="M26" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="27">
+      <c r="N26">
+        <v>5.8520197234703284</v>
+      </c>
+      <c r="O26">
+        <v>51.723289004052667</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>121</v>
       </c>
@@ -3086,8 +3591,14 @@
       <c r="M27" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="28">
+      <c r="N27">
+        <v>6.0293040216680822</v>
+      </c>
+      <c r="O27">
+        <v>51.572383004585568</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>125</v>
       </c>
@@ -3127,8 +3638,14 @@
       <c r="M28" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="29">
+      <c r="N28">
+        <v>5.0203709281979521</v>
+      </c>
+      <c r="O28">
+        <v>51.593077007448692</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>129</v>
       </c>
@@ -3154,7 +3671,7 @@
         <v>18</v>
       </c>
       <c r="I29">
-        <v>9.460000000000001</v>
+        <v>9.4600000000000009</v>
       </c>
       <c r="J29">
         <v>40119.86</v>
@@ -3168,8 +3685,14 @@
       <c r="M29" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="30">
+      <c r="N29">
+        <v>5.4516854238217984</v>
+      </c>
+      <c r="O29">
+        <v>51.450561007503318</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>133</v>
       </c>
@@ -3195,7 +3718,7 @@
         <v>24</v>
       </c>
       <c r="I30">
-        <v>4.888</v>
+        <v>4.8879999999999999</v>
       </c>
       <c r="J30">
         <v>39104</v>
@@ -3209,8 +3732,14 @@
       <c r="M30" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="31">
+      <c r="N30">
+        <v>5.0582895275370596</v>
+      </c>
+      <c r="O30">
+        <v>51.606745006728353</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>136</v>
       </c>
@@ -3236,10 +3765,10 @@
         <v>18</v>
       </c>
       <c r="I31">
-        <v>8.800000000000001</v>
+        <v>8.8000000000000025</v>
       </c>
       <c r="J31">
-        <v>38975.2</v>
+        <v>38975.199999999997</v>
       </c>
       <c r="K31" t="s">
         <v>19</v>
@@ -3250,8 +3779,14 @@
       <c r="M31" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="32">
+      <c r="N31">
+        <v>5.4338671262057243</v>
+      </c>
+      <c r="O31">
+        <v>51.650300005913678</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>140</v>
       </c>
@@ -3277,7 +3812,7 @@
         <v>18</v>
       </c>
       <c r="I32">
-        <v>4.98</v>
+        <v>4.9800000000000004</v>
       </c>
       <c r="J32">
         <v>37350</v>
@@ -3291,8 +3826,14 @@
       <c r="M32" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="33">
+      <c r="N32">
+        <v>5.9080012223591698</v>
+      </c>
+      <c r="O32">
+        <v>51.561437005376362</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>144</v>
       </c>
@@ -3332,8 +3873,14 @@
       <c r="M33" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="34">
+      <c r="N33">
+        <v>5.0790369285614982</v>
+      </c>
+      <c r="O33">
+        <v>51.709239006338073</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>148</v>
       </c>
@@ -3359,7 +3906,7 @@
         <v>24</v>
       </c>
       <c r="I34">
-        <v>4.5916</v>
+        <v>4.5915999999999997</v>
       </c>
       <c r="J34">
         <v>36733.11</v>
@@ -3373,8 +3920,14 @@
       <c r="M34" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="35">
+      <c r="N34">
+        <v>5.0790369285614982</v>
+      </c>
+      <c r="O34">
+        <v>51.709239006338073</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>151</v>
       </c>
@@ -3414,8 +3967,14 @@
       <c r="M35" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="36">
+      <c r="N35">
+        <v>4.9213952292441396</v>
+      </c>
+      <c r="O35">
+        <v>51.621659006922528</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>155</v>
       </c>
@@ -3441,7 +4000,7 @@
         <v>18</v>
       </c>
       <c r="I36">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="J36">
         <v>34500</v>
@@ -3455,8 +4014,14 @@
       <c r="M36" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="37">
+      <c r="N36">
+        <v>4.929876629076718</v>
+      </c>
+      <c r="O36">
+        <v>51.572970007626722</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>158</v>
       </c>
@@ -3496,8 +4061,14 @@
       <c r="M37" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="38">
+      <c r="N37">
+        <v>4.415466331781972</v>
+      </c>
+      <c r="O37">
+        <v>51.626308008273618</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>161</v>
       </c>
@@ -3537,8 +4108,14 @@
       <c r="M38" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="39">
+      <c r="N38">
+        <v>5.8340759233055017</v>
+      </c>
+      <c r="O38">
+        <v>51.652593004736453</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>165</v>
       </c>
@@ -3578,8 +4155,14 @@
       <c r="M39" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="40">
+      <c r="N39">
+        <v>5.7464412214370144</v>
+      </c>
+      <c r="O39">
+        <v>51.380442007432237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>168</v>
       </c>
@@ -3619,8 +4202,14 @@
       <c r="M40" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="41">
+      <c r="N40">
+        <v>4.7641380297415941</v>
+      </c>
+      <c r="O40">
+        <v>51.616672007893918</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>172</v>
       </c>
@@ -3646,7 +4235,7 @@
         <v>18</v>
       </c>
       <c r="I41">
-        <v>4.808</v>
+        <v>4.8079999999999998</v>
       </c>
       <c r="J41">
         <v>28128.33</v>
@@ -3660,8 +4249,14 @@
       <c r="M41" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="42">
+      <c r="N41">
+        <v>5.1433732268583157</v>
+      </c>
+      <c r="O41">
+        <v>51.468361007522887</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>176</v>
       </c>
@@ -3701,8 +4296,14 @@
       <c r="M42" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="43">
+      <c r="N42">
+        <v>5.8321875230360138</v>
+      </c>
+      <c r="O42">
+        <v>51.671553005053269</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>179</v>
       </c>
@@ -3728,10 +4329,10 @@
         <v>18</v>
       </c>
       <c r="I43">
-        <v>3.389</v>
+        <v>3.3889999999999998</v>
       </c>
       <c r="J43">
-        <v>25830.96</v>
+        <v>25830.959999999999</v>
       </c>
       <c r="K43" t="s">
         <v>19</v>
@@ -3742,8 +4343,14 @@
       <c r="M43" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="44">
+      <c r="N43">
+        <v>5.0582895275370596</v>
+      </c>
+      <c r="O43">
+        <v>51.606745006728353</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>182</v>
       </c>
@@ -3769,7 +4376,7 @@
         <v>35</v>
       </c>
       <c r="I44">
-        <v>3.5718</v>
+        <v>3.5718000000000001</v>
       </c>
       <c r="J44">
         <v>25002.54</v>
@@ -3783,8 +4390,14 @@
       <c r="M44" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="45">
+      <c r="N44">
+        <v>5.2505108280112944</v>
+      </c>
+      <c r="O44">
+        <v>51.725030005962701</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>186</v>
       </c>
@@ -3824,8 +4437,14 @@
       <c r="M45" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="46">
+      <c r="N45">
+        <v>5.4338671262057243</v>
+      </c>
+      <c r="O45">
+        <v>51.650300005913678</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>189</v>
       </c>
@@ -3865,8 +4484,14 @@
       <c r="M46" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="47">
+      <c r="N46">
+        <v>5.7227309235375516</v>
+      </c>
+      <c r="O46">
+        <v>51.657796004892496</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>193</v>
       </c>
@@ -3906,8 +4531,14 @@
       <c r="M47" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="48">
+      <c r="N47">
+        <v>5.0582895275370596</v>
+      </c>
+      <c r="O47">
+        <v>51.606745006728353</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>196</v>
       </c>
@@ -3933,10 +4564,10 @@
         <v>18</v>
       </c>
       <c r="I48">
-        <v>4.021</v>
+        <v>4.0209999999999999</v>
       </c>
       <c r="J48">
-        <v>23542.96</v>
+        <v>23542.959999999999</v>
       </c>
       <c r="K48" t="s">
         <v>19</v>
@@ -3947,8 +4578,14 @@
       <c r="M48" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="49">
+      <c r="N48">
+        <v>5.8340759233055017</v>
+      </c>
+      <c r="O48">
+        <v>51.652593004736453</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>199</v>
       </c>
@@ -3974,7 +4611,7 @@
         <v>18</v>
       </c>
       <c r="I49">
-        <v>3.253</v>
+        <v>3.2530000000000001</v>
       </c>
       <c r="J49">
         <v>19000</v>
@@ -3988,8 +4625,14 @@
       <c r="M49" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="50">
+      <c r="N49">
+        <v>5.5311079245482677</v>
+      </c>
+      <c r="O49">
+        <v>51.639375005415893</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>203</v>
       </c>
@@ -4029,8 +4672,14 @@
       <c r="M50" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="51">
+      <c r="N50">
+        <v>5.0203709281979521</v>
+      </c>
+      <c r="O50">
+        <v>51.593077007448692</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>206</v>
       </c>
@@ -4056,7 +4705,7 @@
         <v>18</v>
       </c>
       <c r="I51">
-        <v>3.253</v>
+        <v>3.2530000000000001</v>
       </c>
       <c r="J51">
         <v>18523.61</v>
@@ -4070,8 +4719,14 @@
       <c r="M51" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="52">
+      <c r="N51">
+        <v>5.5311079245482677</v>
+      </c>
+      <c r="O51">
+        <v>51.639375005415893</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>209</v>
       </c>
@@ -4111,8 +4766,14 @@
       <c r="M52" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="53">
+      <c r="N52">
+        <v>5.745882323566744</v>
+      </c>
+      <c r="O52">
+        <v>51.662508004962532</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>212</v>
       </c>
@@ -4138,7 +4799,7 @@
         <v>18</v>
       </c>
       <c r="I53">
-        <v>2.934</v>
+        <v>2.9340000000000002</v>
       </c>
       <c r="J53">
         <v>17178.57</v>
@@ -4152,8 +4813,14 @@
       <c r="M53" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="54">
+      <c r="N53">
+        <v>5.6689008224254378</v>
+      </c>
+      <c r="O53">
+        <v>51.451485007101347</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>216</v>
       </c>
@@ -4182,7 +4849,7 @@
         <v>2.839</v>
       </c>
       <c r="J54">
-        <v>16622.35</v>
+        <v>16622.349999999999</v>
       </c>
       <c r="K54" t="s">
         <v>19</v>
@@ -4193,8 +4860,14 @@
       <c r="M54" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="55">
+      <c r="N54">
+        <v>5.4525330244423023</v>
+      </c>
+      <c r="O54">
+        <v>51.510426007162309</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>219</v>
       </c>
@@ -4234,8 +4907,14 @@
       <c r="M55" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="56">
+      <c r="N55">
+        <v>5.2649497261974458</v>
+      </c>
+      <c r="O55">
+        <v>51.531518006822857</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>223</v>
       </c>
@@ -4275,8 +4954,14 @@
       <c r="M56" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="57">
+      <c r="N56">
+        <v>4.6175266309465197</v>
+      </c>
+      <c r="O56">
+        <v>51.699610007199787</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>227</v>
       </c>
@@ -4302,7 +4987,7 @@
         <v>24</v>
       </c>
       <c r="I57">
-        <v>2.9308</v>
+        <v>2.9308000000000001</v>
       </c>
       <c r="J57">
         <v>15234.74</v>
@@ -4316,8 +5001,14 @@
       <c r="M57" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="58">
+      <c r="N57">
+        <v>4.9738212282179743</v>
+      </c>
+      <c r="O57">
+        <v>51.488235008074767</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>231</v>
       </c>
@@ -4357,8 +5048,14 @@
       <c r="M58" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="59">
+      <c r="N58">
+        <v>4.3308014319722963</v>
+      </c>
+      <c r="O58">
+        <v>51.548453009168163</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>235</v>
       </c>
@@ -4384,7 +5081,7 @@
         <v>18</v>
       </c>
       <c r="I59">
-        <v>2.404</v>
+        <v>2.4039999999999999</v>
       </c>
       <c r="J59">
         <v>14075.42</v>
@@ -4398,8 +5095,14 @@
       <c r="M59" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="60">
+      <c r="N59">
+        <v>5.6886672222774743</v>
+      </c>
+      <c r="O59">
+        <v>51.439235006350032</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>239</v>
       </c>
@@ -4425,7 +5128,7 @@
         <v>35</v>
       </c>
       <c r="I60">
-        <v>7.2244</v>
+        <v>7.2244000000000002</v>
       </c>
       <c r="J60">
         <v>14047.39</v>
@@ -4439,8 +5142,14 @@
       <c r="M60" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="61">
+      <c r="N60">
+        <v>5.2787241278101504</v>
+      </c>
+      <c r="O60">
+        <v>51.702039006257053</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>243</v>
       </c>
@@ -4480,8 +5189,14 @@
       <c r="M61" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="62">
+      <c r="N61">
+        <v>5.8091119232253581</v>
+      </c>
+      <c r="O61">
+        <v>51.661918005103587</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>247</v>
       </c>
@@ -4507,7 +5222,7 @@
         <v>18</v>
       </c>
       <c r="I62">
-        <v>2.267</v>
+        <v>2.2669999999999999</v>
       </c>
       <c r="J62">
         <v>13263.06</v>
@@ -4521,8 +5236,14 @@
       <c r="M62" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="63">
+      <c r="N62">
+        <v>5.729005622291492</v>
+      </c>
+      <c r="O62">
+        <v>51.510464006293638</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>251</v>
       </c>
@@ -4562,8 +5283,14 @@
       <c r="M63" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="64">
+      <c r="N63">
+        <v>5.4525330244423023</v>
+      </c>
+      <c r="O63">
+        <v>51.510426007162309</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>254</v>
       </c>
@@ -4603,8 +5330,14 @@
       <c r="M64" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="65">
+      <c r="N64">
+        <v>5.4525330244423023</v>
+      </c>
+      <c r="O64">
+        <v>51.510426007162309</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>257</v>
       </c>
@@ -4644,8 +5377,14 @@
       <c r="M65" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="66">
+      <c r="N65">
+        <v>4.7641380297415941</v>
+      </c>
+      <c r="O65">
+        <v>51.616672007893918</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>260</v>
       </c>
@@ -4685,8 +5424,14 @@
       <c r="M66" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="67">
+      <c r="N66">
+        <v>5.5190632244014424</v>
+      </c>
+      <c r="O66">
+        <v>51.613639006052757</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>264</v>
       </c>
@@ -4726,8 +5471,14 @@
       <c r="M67" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="68">
+      <c r="N67">
+        <v>5.3209054255591504</v>
+      </c>
+      <c r="O67">
+        <v>51.578835006486521</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>268</v>
       </c>
@@ -4753,7 +5504,7 @@
         <v>18</v>
       </c>
       <c r="I68">
-        <v>1.912</v>
+        <v>1.9119999999999999</v>
       </c>
       <c r="J68">
         <v>10910</v>
@@ -4767,8 +5518,14 @@
       <c r="M68" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="69">
+      <c r="N68">
+        <v>5.729005622291492</v>
+      </c>
+      <c r="O68">
+        <v>51.510464006293638</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>271</v>
       </c>
@@ -4808,8 +5565,14 @@
       <c r="M69" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="70">
+      <c r="N69">
+        <v>4.8683228285940583</v>
+      </c>
+      <c r="O69">
+        <v>51.583747007503689</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>275</v>
       </c>
@@ -4849,8 +5612,14 @@
       <c r="M70" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="71">
+      <c r="N70">
+        <v>5.4525330244423023</v>
+      </c>
+      <c r="O70">
+        <v>51.510426007162309</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>278</v>
       </c>
@@ -4876,10 +5645,10 @@
         <v>24</v>
       </c>
       <c r="I71">
-        <v>1.2212</v>
+        <v>1.2212000000000001</v>
       </c>
       <c r="J71">
-        <v>9769.450000000001</v>
+        <v>9769.4500000000007</v>
       </c>
       <c r="K71" t="s">
         <v>25</v>
@@ -4890,8 +5659,14 @@
       <c r="M71" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="72">
+      <c r="N71">
+        <v>5.4858264253204778</v>
+      </c>
+      <c r="O71">
+        <v>51.578329006285159</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>282</v>
       </c>
@@ -4931,8 +5706,14 @@
       <c r="M72" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="73">
+      <c r="N72">
+        <v>5.3931504249502016</v>
+      </c>
+      <c r="O72">
+        <v>51.44382600731349</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>286</v>
       </c>
@@ -4972,8 +5753,14 @@
       <c r="M73" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="74">
+      <c r="N73">
+        <v>4.6175266309465197</v>
+      </c>
+      <c r="O73">
+        <v>51.699610007199787</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>289</v>
       </c>
@@ -4999,7 +5786,7 @@
         <v>24</v>
       </c>
       <c r="I74">
-        <v>1.1822</v>
+        <v>1.1821999999999999</v>
       </c>
       <c r="J74">
         <v>9457</v>
@@ -5013,8 +5800,14 @@
       <c r="M74" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="75">
+      <c r="N74">
+        <v>4.9738212282179743</v>
+      </c>
+      <c r="O74">
+        <v>51.488235008074767</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>292</v>
       </c>
@@ -5040,10 +5833,10 @@
         <v>18</v>
       </c>
       <c r="I75">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="J75">
-        <v>9330.139999999999</v>
+        <v>9330.14</v>
       </c>
       <c r="K75" t="s">
         <v>19</v>
@@ -5054,8 +5847,14 @@
       <c r="M75" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="76">
+      <c r="N75">
+        <v>5.6214727250264076</v>
+      </c>
+      <c r="O75">
+        <v>51.637463005762207</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>296</v>
       </c>
@@ -5095,8 +5894,14 @@
       <c r="M76" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="77">
+      <c r="N76">
+        <v>5.2649497261974458</v>
+      </c>
+      <c r="O76">
+        <v>51.531518006822857</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>299</v>
       </c>
@@ -5122,7 +5927,7 @@
         <v>18</v>
       </c>
       <c r="I77">
-        <v>1.065</v>
+        <v>1.0649999999999999</v>
       </c>
       <c r="J77">
         <v>8520</v>
@@ -5136,8 +5941,14 @@
       <c r="M77" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="78">
+      <c r="N77">
+        <v>5.2649497261974458</v>
+      </c>
+      <c r="O77">
+        <v>51.531518006822857</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>302</v>
       </c>
@@ -5163,7 +5974,7 @@
         <v>18</v>
       </c>
       <c r="I78">
-        <v>2.725</v>
+        <v>2.7250000000000001</v>
       </c>
       <c r="J78">
         <v>7400</v>
@@ -5177,8 +5988,14 @@
       <c r="M78" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="79">
+      <c r="N78">
+        <v>5.4525330244423023</v>
+      </c>
+      <c r="O78">
+        <v>51.510426007162309</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>305</v>
       </c>
@@ -5218,8 +6035,14 @@
       <c r="M79" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="80">
+      <c r="N79">
+        <v>5.6085040242033841</v>
+      </c>
+      <c r="O79">
+        <v>51.518046006767719</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>309</v>
       </c>
@@ -5245,7 +6068,7 @@
         <v>18</v>
       </c>
       <c r="I80">
-        <v>18.132</v>
+        <v>18.132000000000001</v>
       </c>
       <c r="J80">
         <v>6904</v>
@@ -5259,8 +6082,14 @@
       <c r="M80" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="81">
+      <c r="N80">
+        <v>4.5798263317076797</v>
+      </c>
+      <c r="O80">
+        <v>51.682658008186763</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>312</v>
       </c>
@@ -5286,7 +6115,7 @@
         <v>35</v>
       </c>
       <c r="I81">
-        <v>0.972</v>
+        <v>0.97199999999999998</v>
       </c>
       <c r="J81">
         <v>6787.52</v>
@@ -5300,8 +6129,14 @@
       <c r="M81" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="82">
+      <c r="N81">
+        <v>4.9258800284363362</v>
+      </c>
+      <c r="O81">
+        <v>51.616502007519422</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>316</v>
       </c>
@@ -5341,8 +6176,14 @@
       <c r="M82" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="83">
+      <c r="N82">
+        <v>5.2006076265049019</v>
+      </c>
+      <c r="O82">
+        <v>51.608697006573983</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>320</v>
       </c>
@@ -5382,8 +6223,14 @@
       <c r="M83" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="84">
+      <c r="N83">
+        <v>4.4841947318591613</v>
+      </c>
+      <c r="O83">
+        <v>51.563709009003773</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>324</v>
       </c>
@@ -5409,7 +6256,7 @@
         <v>18</v>
       </c>
       <c r="I84">
-        <v>1.011</v>
+        <v>1.0109999999999999</v>
       </c>
       <c r="J84">
         <v>5919</v>
@@ -5423,8 +6270,14 @@
       <c r="M84" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="85">
+      <c r="N84">
+        <v>5.6176809223331201</v>
+      </c>
+      <c r="O84">
+        <v>51.365481007483567</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>328</v>
       </c>
@@ -5464,8 +6317,14 @@
       <c r="M85" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="86">
+      <c r="N85">
+        <v>5.4255240267896836</v>
+      </c>
+      <c r="O85">
+        <v>51.800428004912277</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>332</v>
       </c>
@@ -5491,7 +6350,7 @@
         <v>35</v>
       </c>
       <c r="I86">
-        <v>1.404</v>
+        <v>1.4039999999999999</v>
       </c>
       <c r="J86">
         <v>5616</v>
@@ -5505,8 +6364,14 @@
       <c r="M86" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="87">
+      <c r="N86">
+        <v>5.4904512271643178</v>
+      </c>
+      <c r="O86">
+        <v>51.815036004777362</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>336</v>
       </c>
@@ -5532,7 +6397,7 @@
         <v>18</v>
       </c>
       <c r="I87">
-        <v>0.959</v>
+        <v>0.95899999999999996</v>
       </c>
       <c r="J87">
         <v>5614.95</v>
@@ -5546,8 +6411,14 @@
       <c r="M87" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="88">
+      <c r="N87">
+        <v>5.6176809223331201</v>
+      </c>
+      <c r="O87">
+        <v>51.365481007483567</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>339</v>
       </c>
@@ -5587,8 +6458,14 @@
       <c r="M88" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="89">
+      <c r="N88">
+        <v>5.5511078232917299</v>
+      </c>
+      <c r="O88">
+        <v>51.282660008388312</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>343</v>
       </c>
@@ -5628,8 +6505,14 @@
       <c r="M89" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="90">
+      <c r="N89">
+        <v>5.5332863246330781</v>
+      </c>
+      <c r="O89">
+        <v>51.649776005661671</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>347</v>
       </c>
@@ -5669,8 +6552,14 @@
       <c r="M90" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="91">
+      <c r="N90">
+        <v>5.9933840214056824</v>
+      </c>
+      <c r="O90">
+        <v>51.594166004702643</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>351</v>
       </c>
@@ -5710,8 +6599,14 @@
       <c r="M91" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="92">
+      <c r="N91">
+        <v>5.0666867280288459</v>
+      </c>
+      <c r="O91">
+        <v>51.517501007282092</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>355</v>
       </c>
@@ -5737,7 +6632,7 @@
         <v>18</v>
       </c>
       <c r="I92">
-        <v>0.8129999999999999</v>
+        <v>0.81299999999999994</v>
       </c>
       <c r="J92">
         <v>4658.33</v>
@@ -5751,8 +6646,14 @@
       <c r="M92" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="93">
+      <c r="N92">
+        <v>5.729005622291492</v>
+      </c>
+      <c r="O92">
+        <v>51.510464006293638</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>358</v>
       </c>
@@ -5778,7 +6679,7 @@
         <v>18</v>
       </c>
       <c r="I93">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J93">
         <v>4400</v>
@@ -5792,8 +6693,14 @@
       <c r="M93" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="94">
+      <c r="N93">
+        <v>5.1624719259284158</v>
+      </c>
+      <c r="O93">
+        <v>51.346288009047242</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>362</v>
       </c>
@@ -5833,8 +6740,14 @@
       <c r="M94" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="95">
+      <c r="N94">
+        <v>5.4093139244684458</v>
+      </c>
+      <c r="O94">
+        <v>51.304664008521783</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>366</v>
       </c>
@@ -5874,8 +6787,14 @@
       <c r="M95" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="96">
+      <c r="N95">
+        <v>5.3028755249775541</v>
+      </c>
+      <c r="O95">
+        <v>51.495347007223877</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>370</v>
       </c>
@@ -5915,8 +6834,14 @@
       <c r="M96" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="97">
+      <c r="N96">
+        <v>5.9049135226754776</v>
+      </c>
+      <c r="O96">
+        <v>51.601744005207422</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>374</v>
       </c>
@@ -5956,8 +6881,14 @@
       <c r="M97" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="98">
+      <c r="N97">
+        <v>5.0489743275599004</v>
+      </c>
+      <c r="O97">
+        <v>51.627435006665543</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>378</v>
       </c>
@@ -5997,8 +6928,14 @@
       <c r="M98" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="99">
+      <c r="N98">
+        <v>5.2568516256546456</v>
+      </c>
+      <c r="O98">
+        <v>51.456074007643089</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>382</v>
       </c>
@@ -6038,8 +6975,14 @@
       <c r="M99" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="100">
+      <c r="N99">
+        <v>4.2982021321207711</v>
+      </c>
+      <c r="O99">
+        <v>51.431116010206402</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>386</v>
       </c>
@@ -6079,8 +7022,14 @@
       <c r="M100" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="101">
+      <c r="N100">
+        <v>5.4649133250787019</v>
+      </c>
+      <c r="O100">
+        <v>51.612930006057248</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>390</v>
       </c>
@@ -6120,8 +7069,14 @@
       <c r="M101" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="102">
+      <c r="N101">
+        <v>5.9080012223591698</v>
+      </c>
+      <c r="O101">
+        <v>51.561437005376362</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>393</v>
       </c>
@@ -6161,8 +7116,14 @@
       <c r="M102" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="103">
+      <c r="N102">
+        <v>5.4224135265495779</v>
+      </c>
+      <c r="O102">
+        <v>51.674294005863459</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>397</v>
       </c>
@@ -6202,8 +7163,14 @@
       <c r="M103" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="104">
+      <c r="N103">
+        <v>5.8971000225978658</v>
+      </c>
+      <c r="O103">
+        <v>51.651806004914476</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>401</v>
       </c>
@@ -6229,7 +7196,7 @@
         <v>35</v>
       </c>
       <c r="I104">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J104">
         <v>2833.33</v>
@@ -6243,8 +7210,14 @@
       <c r="M104" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="105">
+      <c r="N104">
+        <v>4.7536546295878237</v>
+      </c>
+      <c r="O104">
+        <v>51.58364900837956</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>405</v>
       </c>
@@ -6284,8 +7257,14 @@
       <c r="M105" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="106">
+      <c r="N105">
+        <v>5.4255240267896836</v>
+      </c>
+      <c r="O105">
+        <v>51.800428004912277</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>408</v>
       </c>
@@ -6325,8 +7304,14 @@
       <c r="M106" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="107">
+      <c r="N106">
+        <v>5.5181828260405936</v>
+      </c>
+      <c r="O106">
+        <v>51.783197004535857</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>412</v>
       </c>
@@ -6366,8 +7351,14 @@
       <c r="M107" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="108">
+      <c r="N107">
+        <v>5.8022759218170981</v>
+      </c>
+      <c r="O107">
+        <v>51.449114006472144</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>416</v>
       </c>
@@ -6407,8 +7398,14 @@
       <c r="M108" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="109">
+      <c r="N108">
+        <v>5.3686063252482583</v>
+      </c>
+      <c r="O108">
+        <v>51.528067007155613</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>420</v>
       </c>
@@ -6448,8 +7445,14 @@
       <c r="M109" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="110">
+      <c r="N109">
+        <v>4.5966706298697337</v>
+      </c>
+      <c r="O109">
+        <v>51.528347009071801</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>424</v>
       </c>
@@ -6489,8 +7492,14 @@
       <c r="M110" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="111">
+      <c r="N110">
+        <v>5.8623934226941081</v>
+      </c>
+      <c r="O110">
+        <v>51.693330004806711</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>428</v>
       </c>
@@ -6516,7 +7525,7 @@
         <v>35</v>
       </c>
       <c r="I111">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J111">
         <v>2200</v>
@@ -6530,8 +7539,14 @@
       <c r="M111" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="112">
+      <c r="N111">
+        <v>5.7342698245608243</v>
+      </c>
+      <c r="O111">
+        <v>51.748678004189223</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>432</v>
       </c>
@@ -6557,7 +7572,7 @@
         <v>435</v>
       </c>
       <c r="I112">
-        <v>3.4027</v>
+        <v>3.4026999999999998</v>
       </c>
       <c r="J112">
         <v>2041.62</v>
@@ -6571,8 +7586,14 @@
       <c r="M112" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="113">
+      <c r="N112">
+        <v>5.0548964280419284</v>
+      </c>
+      <c r="O112">
+        <v>51.697526006725838</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>438</v>
       </c>
@@ -6612,8 +7633,14 @@
       <c r="M113" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="114">
+      <c r="N113">
+        <v>5.3866167244326002</v>
+      </c>
+      <c r="O113">
+        <v>51.359383008399888</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>442</v>
       </c>
@@ -6653,8 +7680,14 @@
       <c r="M114" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="115">
+      <c r="N114">
+        <v>5.8537855221222221</v>
+      </c>
+      <c r="O114">
+        <v>51.579281005237803</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>446</v>
       </c>
@@ -6694,8 +7727,14 @@
       <c r="M115" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="116">
+      <c r="N115">
+        <v>4.7744003310325436</v>
+      </c>
+      <c r="O115">
+        <v>51.763477006836659</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>450</v>
       </c>
@@ -6735,8 +7774,14 @@
       <c r="M116" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="117">
+      <c r="N116">
+        <v>5.6766927238679799</v>
+      </c>
+      <c r="O116">
+        <v>51.606897005363493</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>454</v>
       </c>
@@ -6776,8 +7821,14 @@
       <c r="M117" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="118">
+      <c r="N117">
+        <v>4.5716246304739858</v>
+      </c>
+      <c r="O117">
+        <v>51.455813009664801</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>458</v>
       </c>
@@ -6817,8 +7868,14 @@
       <c r="M118" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="119">
+      <c r="N118">
+        <v>5.133958228681216</v>
+      </c>
+      <c r="O118">
+        <v>51.704748006420829</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>462</v>
       </c>
@@ -6858,8 +7915,14 @@
       <c r="M119" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="120">
+      <c r="N119">
+        <v>5.045592527795054</v>
+      </c>
+      <c r="O119">
+        <v>51.646016007034177</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>466</v>
       </c>
@@ -6899,8 +7962,14 @@
       <c r="M120" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="121">
+      <c r="N120">
+        <v>5.7135331228282098</v>
+      </c>
+      <c r="O120">
+        <v>51.458824006416897</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>470</v>
       </c>
@@ -6940,8 +8009,14 @@
       <c r="M121" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="122">
+      <c r="N121">
+        <v>4.8020867303899921</v>
+      </c>
+      <c r="O121">
+        <v>51.683287006773782</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>473</v>
       </c>
@@ -6981,8 +8056,14 @@
       <c r="M122" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="123">
+      <c r="N122">
+        <v>5.2592275247316023</v>
+      </c>
+      <c r="O122">
+        <v>51.353508008608031</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>477</v>
       </c>
@@ -7011,7 +8092,7 @@
         <v>0.74</v>
       </c>
       <c r="J123">
-        <v>1161.11</v>
+        <v>1161.1099999999999</v>
       </c>
       <c r="K123" t="s">
         <v>19</v>
@@ -7022,8 +8103,14 @@
       <c r="M123" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="124">
+      <c r="N123">
+        <v>5.2505108280112944</v>
+      </c>
+      <c r="O123">
+        <v>51.725030005962701</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>480</v>
       </c>
@@ -7063,8 +8150,14 @@
       <c r="M124" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="125">
+      <c r="N124">
+        <v>5.5269349252131921</v>
+      </c>
+      <c r="O124">
+        <v>51.666500005648899</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>484</v>
       </c>
@@ -7104,8 +8197,14 @@
       <c r="M125" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="126">
+      <c r="N125">
+        <v>5.1136475265664796</v>
+      </c>
+      <c r="O125">
+        <v>51.390945008342833</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>488</v>
       </c>
@@ -7145,8 +8244,14 @@
       <c r="M126" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="127">
+      <c r="N126">
+        <v>5.7554273215012621</v>
+      </c>
+      <c r="O126">
+        <v>51.347271007231043</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>492</v>
       </c>
@@ -7186,8 +8291,14 @@
       <c r="M127" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="128">
+      <c r="N127">
+        <v>5.7554273215012621</v>
+      </c>
+      <c r="O127">
+        <v>51.347271007231043</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>495</v>
       </c>
@@ -7227,8 +8338,14 @@
       <c r="M128" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="129">
+      <c r="N128">
+        <v>4.284005132327235</v>
+      </c>
+      <c r="O128">
+        <v>51.428614010394931</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>499</v>
       </c>
@@ -7268,8 +8385,14 @@
       <c r="M129" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="130">
+      <c r="N129">
+        <v>4.5815631309439677</v>
+      </c>
+      <c r="O129">
+        <v>51.584578008786039</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>503</v>
       </c>
@@ -7309,8 +8432,14 @@
       <c r="M130" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="131">
+      <c r="N130">
+        <v>5.7217224217853699</v>
+      </c>
+      <c r="O130">
+        <v>51.364958006781038</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>507</v>
       </c>
@@ -7350,8 +8479,14 @@
       <c r="M131" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="132">
+      <c r="N131">
+        <v>5.5542164244240624</v>
+      </c>
+      <c r="O131">
+        <v>51.448762006747323</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>511</v>
       </c>
@@ -7377,7 +8512,7 @@
         <v>18</v>
       </c>
       <c r="I132">
-        <v>0.138</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="J132">
         <v>790.83</v>
@@ -7391,8 +8526,14 @@
       <c r="M132" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="133">
+      <c r="N132">
+        <v>5.4512921239569119</v>
+      </c>
+      <c r="O132">
+        <v>51.316161008380142</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>515</v>
       </c>
@@ -7432,8 +8573,14 @@
       <c r="M133" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="134">
+      <c r="N133">
+        <v>5.3912458268950756</v>
+      </c>
+      <c r="O133">
+        <v>51.778375004778958</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>519</v>
       </c>
@@ -7473,8 +8620,14 @@
       <c r="M134" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="135">
+      <c r="N134">
+        <v>5.7191601237276499</v>
+      </c>
+      <c r="O134">
+        <v>51.642026004858799</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>523</v>
       </c>
@@ -7514,8 +8667,14 @@
       <c r="M135" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="136">
+      <c r="N135">
+        <v>5.4885409253515123</v>
+      </c>
+      <c r="O135">
+        <v>51.658602005827078</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>527</v>
       </c>
@@ -7555,8 +8714,14 @@
       <c r="M136" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="137">
+      <c r="N136">
+        <v>5.4674926253703839</v>
+      </c>
+      <c r="O136">
+        <v>51.563103006745877</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>531</v>
       </c>
@@ -7596,8 +8761,14 @@
       <c r="M137" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="138">
+      <c r="N137">
+        <v>5.7679513230740964</v>
+      </c>
+      <c r="O137">
+        <v>51.511981006423063</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>535</v>
       </c>
@@ -7623,7 +8794,7 @@
         <v>435</v>
       </c>
       <c r="I138">
-        <v>0.494</v>
+        <v>0.49399999999999999</v>
       </c>
       <c r="J138">
         <v>345.8</v>
@@ -7637,8 +8808,14 @@
       <c r="M138" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="139">
+      <c r="N138">
+        <v>5.7050086225159964</v>
+      </c>
+      <c r="O138">
+        <v>51.352914007669042</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>539</v>
       </c>
@@ -7664,7 +8841,7 @@
         <v>435</v>
       </c>
       <c r="I139">
-        <v>0.4928</v>
+        <v>0.49280000000000002</v>
       </c>
       <c r="J139">
         <v>344.96</v>
@@ -7678,8 +8855,14 @@
       <c r="M139" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="140">
+      <c r="N139">
+        <v>5.0485314273802722</v>
+      </c>
+      <c r="O139">
+        <v>51.586678006961442</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>543</v>
       </c>
@@ -7719,8 +8902,14 @@
       <c r="M140" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="141">
+      <c r="N140">
+        <v>5.5315003260124342</v>
+      </c>
+      <c r="O140">
+        <v>51.69526300514012</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>546</v>
       </c>
@@ -7746,10 +8935,10 @@
         <v>435</v>
       </c>
       <c r="I141">
-        <v>0.462</v>
+        <v>0.46200000000000002</v>
       </c>
       <c r="J141">
-        <v>323.4</v>
+        <v>323.39999999999998</v>
       </c>
       <c r="K141" t="s">
         <v>436</v>
@@ -7760,8 +8949,14 @@
       <c r="M141" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="142">
+      <c r="N141">
+        <v>5.6766927238679799</v>
+      </c>
+      <c r="O141">
+        <v>51.606897005363493</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>549</v>
       </c>
@@ -7787,10 +8982,10 @@
         <v>435</v>
       </c>
       <c r="I142">
-        <v>0.448</v>
+        <v>0.44800000000000001</v>
       </c>
       <c r="J142">
-        <v>313.6</v>
+        <v>313.60000000000002</v>
       </c>
       <c r="K142" t="s">
         <v>436</v>
@@ -7801,8 +8996,14 @@
       <c r="M142" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="143">
+      <c r="N142">
+        <v>5.7088964229226864</v>
+      </c>
+      <c r="O142">
+        <v>51.568091005560859</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>553</v>
       </c>
@@ -7828,10 +9029,10 @@
         <v>435</v>
       </c>
       <c r="I143">
-        <v>0.4991</v>
+        <v>0.49909999999999999</v>
       </c>
       <c r="J143">
-        <v>299.46</v>
+        <v>299.45999999999998</v>
       </c>
       <c r="K143" t="s">
         <v>436</v>
@@ -7842,8 +9043,14 @@
       <c r="M143" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="144">
+      <c r="N143">
+        <v>5.4248682237658343</v>
+      </c>
+      <c r="O143">
+        <v>51.410465007959999</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>557</v>
       </c>
@@ -7869,10 +9076,10 @@
         <v>435</v>
       </c>
       <c r="I144">
-        <v>0.4991</v>
+        <v>0.49909999999999999</v>
       </c>
       <c r="J144">
-        <v>299.46</v>
+        <v>299.45999999999998</v>
       </c>
       <c r="K144" t="s">
         <v>436</v>
@@ -7883,8 +9090,14 @@
       <c r="M144" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="145">
+      <c r="N144">
+        <v>5.5048100249083776</v>
+      </c>
+      <c r="O144">
+        <v>51.604775006318313</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>560</v>
       </c>
@@ -7910,10 +9123,10 @@
         <v>435</v>
       </c>
       <c r="I145">
-        <v>0.4991</v>
+        <v>0.49909999999999999</v>
       </c>
       <c r="J145">
-        <v>299.46</v>
+        <v>299.45999999999998</v>
       </c>
       <c r="K145" t="s">
         <v>436</v>
@@ -7924,8 +9137,14 @@
       <c r="M145" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="146">
+      <c r="N145">
+        <v>5.5126980243440684</v>
+      </c>
+      <c r="O145">
+        <v>51.597384005967967</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>562</v>
       </c>
@@ -7951,10 +9170,10 @@
         <v>435</v>
       </c>
       <c r="I146">
-        <v>0.4991</v>
+        <v>0.49909999999999999</v>
       </c>
       <c r="J146">
-        <v>299.46</v>
+        <v>299.45999999999998</v>
       </c>
       <c r="K146" t="s">
         <v>436</v>
@@ -7965,8 +9184,14 @@
       <c r="M146" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="147">
+      <c r="N146">
+        <v>5.7008645235060182</v>
+      </c>
+      <c r="O146">
+        <v>51.602363005366421</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>566</v>
       </c>
@@ -7992,10 +9217,10 @@
         <v>435</v>
       </c>
       <c r="I147">
-        <v>0.4991</v>
+        <v>0.49909999999999999</v>
       </c>
       <c r="J147">
-        <v>299.46</v>
+        <v>299.45999999999998</v>
       </c>
       <c r="K147" t="s">
         <v>436</v>
@@ -8006,8 +9231,14 @@
       <c r="M147" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="148">
+      <c r="N147">
+        <v>5.0664089276604676</v>
+      </c>
+      <c r="O147">
+        <v>51.585599007601317</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>569</v>
       </c>
@@ -8033,10 +9264,10 @@
         <v>435</v>
       </c>
       <c r="I148">
-        <v>0.4991</v>
+        <v>0.49909999999999999</v>
       </c>
       <c r="J148">
-        <v>299.46</v>
+        <v>299.45999999999998</v>
       </c>
       <c r="K148" t="s">
         <v>436</v>
@@ -8047,8 +9278,14 @@
       <c r="M148" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="149">
+      <c r="N148">
+        <v>5.523739024561916</v>
+      </c>
+      <c r="O148">
+        <v>51.601080005766697</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>571</v>
       </c>
@@ -8088,8 +9325,14 @@
       <c r="M149" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="150">
+      <c r="N149">
+        <v>5.5781521241951779</v>
+      </c>
+      <c r="O149">
+        <v>51.540030005852707</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>575</v>
       </c>
@@ -8115,7 +9358,7 @@
         <v>435</v>
       </c>
       <c r="I150">
-        <v>0.3696</v>
+        <v>0.36959999999999998</v>
       </c>
       <c r="J150">
         <v>221.76</v>
@@ -8129,8 +9372,14 @@
       <c r="M150" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="151">
+      <c r="N150">
+        <v>5.0308564293944684</v>
+      </c>
+      <c r="O150">
+        <v>51.697330006209761</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>579</v>
       </c>
@@ -8170,8 +9419,14 @@
       <c r="M151" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="152">
+      <c r="N151">
+        <v>5.523739024561916</v>
+      </c>
+      <c r="O151">
+        <v>51.601080005766697</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>582</v>
       </c>
@@ -8211,8 +9466,14 @@
       <c r="M152" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="153">
+      <c r="N152">
+        <v>5.6932736230548544</v>
+      </c>
+      <c r="O152">
+        <v>51.560063005426343</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>585</v>
       </c>
@@ -8252,8 +9513,14 @@
       <c r="M153" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="154">
+      <c r="N153">
+        <v>5.5126980243440684</v>
+      </c>
+      <c r="O153">
+        <v>51.597384005967967</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>586</v>
       </c>
@@ -8293,8 +9560,14 @@
       <c r="M154" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="155">
+      <c r="N154">
+        <v>5.6653009231387736</v>
+      </c>
+      <c r="O154">
+        <v>51.481677006310491</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>590</v>
       </c>
@@ -8334,8 +9607,14 @@
       <c r="M155" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="156">
+      <c r="N155">
+        <v>4.9539533282614663</v>
+      </c>
+      <c r="O155">
+        <v>51.488004008312693</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>594</v>
       </c>
@@ -8375,8 +9654,14 @@
       <c r="M156" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="157">
+      <c r="N156">
+        <v>4.6386838303636457</v>
+      </c>
+      <c r="O156">
+        <v>51.457135008904451</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>598</v>
       </c>
@@ -8416,8 +9701,14 @@
       <c r="M157" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="158">
+      <c r="N157">
+        <v>5.4105777246760436</v>
+      </c>
+      <c r="O157">
+        <v>51.50028600661711</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>602</v>
       </c>
@@ -8457,8 +9748,14 @@
       <c r="M158" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="159">
+      <c r="N158">
+        <v>5.47257402531715</v>
+      </c>
+      <c r="O158">
+        <v>51.537410006783738</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>606</v>
       </c>
@@ -8484,7 +9781,7 @@
         <v>435</v>
       </c>
       <c r="I159">
-        <v>0.1645</v>
+        <v>0.16450000000000001</v>
       </c>
       <c r="J159">
         <v>115.15</v>
@@ -8498,8 +9795,14 @@
       <c r="M159" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="160">
+      <c r="N159">
+        <v>5.7050086225159964</v>
+      </c>
+      <c r="O159">
+        <v>51.352914007669042</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>609</v>
       </c>
@@ -8539,8 +9842,14 @@
       <c r="M160" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="161">
+      <c r="N160">
+        <v>5.5349208237422003</v>
+      </c>
+      <c r="O160">
+        <v>51.335201008173698</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>613</v>
       </c>
@@ -8566,7 +9875,7 @@
         <v>435</v>
       </c>
       <c r="I161">
-        <v>0.1568</v>
+        <v>0.15679999999999999</v>
       </c>
       <c r="J161">
         <v>109.76</v>
@@ -8580,8 +9889,14 @@
       <c r="M161" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="162">
+      <c r="N161">
+        <v>5.4312486247785916</v>
+      </c>
+      <c r="O161">
+        <v>51.431957007370443</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>617</v>
       </c>
@@ -8621,8 +9936,14 @@
       <c r="M162" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="163">
+      <c r="N162">
+        <v>5.499235826534286</v>
+      </c>
+      <c r="O162">
+        <v>51.734735004900053</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>621</v>
       </c>
@@ -8648,7 +9969,7 @@
         <v>435</v>
       </c>
       <c r="I163">
-        <v>0.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J163">
         <v>98</v>
@@ -8662,8 +9983,14 @@
       <c r="M163" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="164">
+      <c r="N163">
+        <v>4.9658820298231277</v>
+      </c>
+      <c r="O163">
+        <v>51.802632005625902</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>625</v>
       </c>
@@ -8689,7 +10016,7 @@
         <v>435</v>
       </c>
       <c r="I164">
-        <v>0.1456</v>
+        <v>0.14560000000000001</v>
       </c>
       <c r="J164">
         <v>87.36</v>
@@ -8703,8 +10030,14 @@
       <c r="M164" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="165">
+      <c r="N164">
+        <v>5.7798996223467736</v>
+      </c>
+      <c r="O164">
+        <v>51.463734006723101</v>
+      </c>
+    </row>
+    <row r="165" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>629</v>
       </c>
@@ -8730,7 +10063,7 @@
         <v>435</v>
       </c>
       <c r="I165">
-        <v>0.08749999999999999</v>
+        <v>8.7499999999999994E-2</v>
       </c>
       <c r="J165">
         <v>61.25</v>
@@ -8744,7 +10077,17 @@
       <c r="M165" t="s">
         <v>632</v>
       </c>
+      <c r="N165">
+        <v>5.2090760278710917</v>
+      </c>
+      <c r="O165">
+        <v>51.694986006115784</v>
+      </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>